<commit_message>
feat: Teste parametros integracao
</commit_message>
<xml_diff>
--- a/docs/usuarios.xlsx
+++ b/docs/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guiga\Documents\Repositorio_Faculdade\Controla_Facil_Backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6700DE4-77A9-470D-A98F-87518E91B788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA35502D-43FA-4609-A999-534F5113BA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1EAE46C1-DDBF-4172-98F4-E017E6AADE33}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>